<commit_message>
More Items in CIA&ICV
</commit_message>
<xml_diff>
--- a/DataFileSamples/Others/Chemical Index of Alteration.xlsx
+++ b/DataFileSamples/Others/Chemical Index of Alteration.xlsx
@@ -8,17 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cycleuser/Documents/GitHub/GeoPyTool/DataFileSamples/Others/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{05FF176A-4786-D54C-B926-74AF5EC328A9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1F28C170-CC46-FA4F-9D74-2B6A5A4A88E2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="1320" windowWidth="23240" windowHeight="20160" activeTab="2" xr2:uid="{412D788D-48D5-5042-9445-1F4F49743A84}"/>
+    <workbookView xWindow="1340" yWindow="2240" windowWidth="23240" windowHeight="20160" xr2:uid="{412D788D-48D5-5042-9445-1F4F49743A84}"/>
   </bookViews>
   <sheets>
-    <sheet name="工作表3" sheetId="6" r:id="rId1"/>
-    <sheet name="CIA" sheetId="3" r:id="rId2"/>
-    <sheet name="工作表1" sheetId="5" r:id="rId3"/>
-    <sheet name="工作表4" sheetId="4" r:id="rId4"/>
-    <sheet name="工作表2" sheetId="2" r:id="rId5"/>
+    <sheet name="CIA" sheetId="3" r:id="rId1"/>
+    <sheet name="工作表5" sheetId="7" r:id="rId2"/>
+    <sheet name="工作表3" sheetId="6" r:id="rId3"/>
+    <sheet name="工作表1" sheetId="5" r:id="rId4"/>
+    <sheet name="工作表4" sheetId="4" r:id="rId5"/>
+    <sheet name="工作表2" sheetId="2" r:id="rId6"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId7"/>
+  </externalReferences>
   <calcPr calcId="162913" iterateCount="200" iterateDelta="9.9999999999999995E-7" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="104">
   <si>
     <t>Author</t>
   </si>
@@ -566,6 +570,14 @@
     <t>TiO2</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>FeO</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fe3O4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -758,6 +770,489 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="工作表1"/>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Al2O3</v>
+          </cell>
+          <cell r="C1" t="str">
+            <v>BaO</v>
+          </cell>
+          <cell r="D1" t="str">
+            <v>CaO</v>
+          </cell>
+          <cell r="E1" t="str">
+            <v>Cr2O3</v>
+          </cell>
+          <cell r="F1" t="str">
+            <v>TFe2O3</v>
+          </cell>
+          <cell r="G1" t="str">
+            <v>K2O</v>
+          </cell>
+          <cell r="H1" t="str">
+            <v>MgO</v>
+          </cell>
+          <cell r="I1" t="str">
+            <v>MnO</v>
+          </cell>
+          <cell r="J1" t="str">
+            <v>Na2O</v>
+          </cell>
+          <cell r="K1" t="str">
+            <v>P2O5</v>
+          </cell>
+          <cell r="L1" t="str">
+            <v>SiO2</v>
+          </cell>
+          <cell r="M1" t="str">
+            <v>SO3</v>
+          </cell>
+          <cell r="N1" t="str">
+            <v>SrO</v>
+          </cell>
+          <cell r="O1" t="str">
+            <v>TiO2</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>JC-SH-13</v>
+          </cell>
+          <cell r="B2">
+            <v>13.91</v>
+          </cell>
+          <cell r="C2">
+            <v>0.08</v>
+          </cell>
+          <cell r="D2">
+            <v>1.58</v>
+          </cell>
+          <cell r="E2">
+            <v>0.06</v>
+          </cell>
+          <cell r="F2">
+            <v>10.92</v>
+          </cell>
+          <cell r="G2">
+            <v>2.4</v>
+          </cell>
+          <cell r="H2">
+            <v>2.19</v>
+          </cell>
+          <cell r="I2">
+            <v>0.06</v>
+          </cell>
+          <cell r="J2">
+            <v>1.17</v>
+          </cell>
+          <cell r="K2">
+            <v>0.26</v>
+          </cell>
+          <cell r="L2">
+            <v>59.73</v>
+          </cell>
+          <cell r="M2">
+            <v>0.04</v>
+          </cell>
+          <cell r="N2">
+            <v>0.06</v>
+          </cell>
+          <cell r="O2">
+            <v>1.44</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>JC-SH-1</v>
+          </cell>
+          <cell r="B3">
+            <v>10.26</v>
+          </cell>
+          <cell r="C3">
+            <v>0.03</v>
+          </cell>
+          <cell r="D3">
+            <v>0.92</v>
+          </cell>
+          <cell r="E3">
+            <v>0.01</v>
+          </cell>
+          <cell r="F3">
+            <v>2.88</v>
+          </cell>
+          <cell r="G3">
+            <v>1.92</v>
+          </cell>
+          <cell r="H3">
+            <v>0.91</v>
+          </cell>
+          <cell r="I3">
+            <v>0.01</v>
+          </cell>
+          <cell r="J3">
+            <v>1.1200000000000001</v>
+          </cell>
+          <cell r="K3">
+            <v>0.14000000000000001</v>
+          </cell>
+          <cell r="L3">
+            <v>76.95</v>
+          </cell>
+          <cell r="M3">
+            <v>0.01</v>
+          </cell>
+          <cell r="N3">
+            <v>0.01</v>
+          </cell>
+          <cell r="O3">
+            <v>0.73</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>JC-SH-2</v>
+          </cell>
+          <cell r="B4">
+            <v>14.3</v>
+          </cell>
+          <cell r="C4">
+            <v>0.06</v>
+          </cell>
+          <cell r="D4">
+            <v>0.48</v>
+          </cell>
+          <cell r="E4">
+            <v>0.02</v>
+          </cell>
+          <cell r="F4">
+            <v>4.1399999999999997</v>
+          </cell>
+          <cell r="G4">
+            <v>2.95</v>
+          </cell>
+          <cell r="H4">
+            <v>1.5</v>
+          </cell>
+          <cell r="I4">
+            <v>0.04</v>
+          </cell>
+          <cell r="J4">
+            <v>0.91</v>
+          </cell>
+          <cell r="K4">
+            <v>0.12</v>
+          </cell>
+          <cell r="L4">
+            <v>71</v>
+          </cell>
+          <cell r="M4">
+            <v>0.02</v>
+          </cell>
+          <cell r="N4">
+            <v>0.02</v>
+          </cell>
+          <cell r="O4">
+            <v>0.9</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>JC-SH-3</v>
+          </cell>
+          <cell r="B5">
+            <v>17.57</v>
+          </cell>
+          <cell r="C5">
+            <v>0.06</v>
+          </cell>
+          <cell r="D5">
+            <v>10.65</v>
+          </cell>
+          <cell r="E5">
+            <v>0.01</v>
+          </cell>
+          <cell r="F5">
+            <v>5.15</v>
+          </cell>
+          <cell r="G5">
+            <v>3.05</v>
+          </cell>
+          <cell r="H5">
+            <v>1.94</v>
+          </cell>
+          <cell r="I5">
+            <v>0.03</v>
+          </cell>
+          <cell r="J5">
+            <v>0.17</v>
+          </cell>
+          <cell r="K5">
+            <v>0.39</v>
+          </cell>
+          <cell r="L5">
+            <v>41.53</v>
+          </cell>
+          <cell r="M5">
+            <v>0.28000000000000003</v>
+          </cell>
+          <cell r="N5">
+            <v>0.03</v>
+          </cell>
+          <cell r="O5">
+            <v>0.53</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>LM-JSC-1</v>
+          </cell>
+          <cell r="B6">
+            <v>11.68</v>
+          </cell>
+          <cell r="C6">
+            <v>0.03</v>
+          </cell>
+          <cell r="D6">
+            <v>7.0000000000000007E-2</v>
+          </cell>
+          <cell r="E6">
+            <v>0.01</v>
+          </cell>
+          <cell r="F6">
+            <v>5.49</v>
+          </cell>
+          <cell r="G6">
+            <v>3.78</v>
+          </cell>
+          <cell r="H6">
+            <v>0.33</v>
+          </cell>
+          <cell r="I6">
+            <v>0.04</v>
+          </cell>
+          <cell r="J6">
+            <v>7.0000000000000007E-2</v>
+          </cell>
+          <cell r="K6">
+            <v>0.1</v>
+          </cell>
+          <cell r="L6">
+            <v>74.5</v>
+          </cell>
+          <cell r="M6">
+            <v>0.01</v>
+          </cell>
+          <cell r="N6">
+            <v>0.02</v>
+          </cell>
+          <cell r="O6">
+            <v>0.36</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>LM-JSC-3</v>
+          </cell>
+          <cell r="B7">
+            <v>10.1</v>
+          </cell>
+          <cell r="C7">
+            <v>0.01</v>
+          </cell>
+          <cell r="D7">
+            <v>1.32</v>
+          </cell>
+          <cell r="E7">
+            <v>0.01</v>
+          </cell>
+          <cell r="F7">
+            <v>2.69</v>
+          </cell>
+          <cell r="G7">
+            <v>2.77</v>
+          </cell>
+          <cell r="H7">
+            <v>0.67</v>
+          </cell>
+          <cell r="I7">
+            <v>0.03</v>
+          </cell>
+          <cell r="J7">
+            <v>0.04</v>
+          </cell>
+          <cell r="K7">
+            <v>0.14000000000000001</v>
+          </cell>
+          <cell r="L7">
+            <v>76.790000000000006</v>
+          </cell>
+          <cell r="M7">
+            <v>0.01</v>
+          </cell>
+          <cell r="N7">
+            <v>0.01</v>
+          </cell>
+          <cell r="O7">
+            <v>0.41</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>JC-JSC-1</v>
+          </cell>
+          <cell r="B8">
+            <v>5.76</v>
+          </cell>
+          <cell r="C8">
+            <v>0.02</v>
+          </cell>
+          <cell r="D8">
+            <v>0.02</v>
+          </cell>
+          <cell r="E8">
+            <v>0.01</v>
+          </cell>
+          <cell r="F8">
+            <v>4.29</v>
+          </cell>
+          <cell r="G8">
+            <v>1.9</v>
+          </cell>
+          <cell r="H8">
+            <v>0.15</v>
+          </cell>
+          <cell r="I8">
+            <v>0.05</v>
+          </cell>
+          <cell r="J8">
+            <v>0.04</v>
+          </cell>
+          <cell r="K8">
+            <v>0.06</v>
+          </cell>
+          <cell r="L8">
+            <v>85.21</v>
+          </cell>
+          <cell r="M8">
+            <v>0.02</v>
+          </cell>
+          <cell r="N8">
+            <v>0.01</v>
+          </cell>
+          <cell r="O8">
+            <v>0.21</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>JC-BXS-9</v>
+          </cell>
+          <cell r="B9">
+            <v>12.3</v>
+          </cell>
+          <cell r="C9">
+            <v>0.02</v>
+          </cell>
+          <cell r="D9">
+            <v>1.1399999999999999</v>
+          </cell>
+          <cell r="E9">
+            <v>0.01</v>
+          </cell>
+          <cell r="F9">
+            <v>4.3099999999999996</v>
+          </cell>
+          <cell r="G9">
+            <v>2.1</v>
+          </cell>
+          <cell r="H9">
+            <v>0.55000000000000004</v>
+          </cell>
+          <cell r="I9">
+            <v>0.04</v>
+          </cell>
+          <cell r="J9">
+            <v>0.08</v>
+          </cell>
+          <cell r="K9">
+            <v>0.18</v>
+          </cell>
+          <cell r="L9">
+            <v>73.650000000000006</v>
+          </cell>
+          <cell r="M9">
+            <v>0.04</v>
+          </cell>
+          <cell r="N9">
+            <v>0.03</v>
+          </cell>
+          <cell r="O9">
+            <v>0.65</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10" t="str">
+            <v>JC-BXS-1</v>
+          </cell>
+          <cell r="B10">
+            <v>15.18</v>
+          </cell>
+          <cell r="C10">
+            <v>0.03</v>
+          </cell>
+          <cell r="D10">
+            <v>0.14000000000000001</v>
+          </cell>
+          <cell r="E10">
+            <v>0.01</v>
+          </cell>
+          <cell r="F10">
+            <v>4.74</v>
+          </cell>
+          <cell r="G10">
+            <v>2.99</v>
+          </cell>
+          <cell r="H10">
+            <v>0.59</v>
+          </cell>
+          <cell r="I10">
+            <v>0.01</v>
+          </cell>
+          <cell r="J10">
+            <v>0.14000000000000001</v>
+          </cell>
+          <cell r="K10">
+            <v>0.11</v>
+          </cell>
+          <cell r="L10">
+            <v>70.86</v>
+          </cell>
+          <cell r="M10">
+            <v>0.01</v>
+          </cell>
+          <cell r="N10">
+            <v>0.05</v>
+          </cell>
+          <cell r="O10">
+            <v>0.91</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1056,16 +1551,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AD2A2BA-2BA1-284D-B683-050BFEF75A5C}">
-  <dimension ref="A1:K5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7DC8ABB-61B9-4E49-970C-882DDCAD30FD}">
+  <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:K5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="A8:O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>93</v>
       </c>
@@ -1079,28 +1574,35 @@
         <v>98</v>
       </c>
       <c r="E1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>99</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>100</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>95</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>101</v>
       </c>
+      <c r="N1" s="6"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:14">
       <c r="A2" s="13" t="s">
         <v>89</v>
       </c>
@@ -1114,28 +1616,35 @@
         <v>0.75</v>
       </c>
       <c r="E2">
+        <v>0.75</v>
+      </c>
+      <c r="F2">
+        <v>0.75</v>
+      </c>
+      <c r="G2">
         <v>14.68</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>21.54</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>0.44</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>1.39</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>0.21</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>0.04</v>
       </c>
-      <c r="K2">
+      <c r="M2">
         <v>0.18</v>
       </c>
+      <c r="N2" s="6"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:14">
       <c r="A3" s="13" t="s">
         <v>90</v>
       </c>
@@ -1149,28 +1658,35 @@
         <v>1.92</v>
       </c>
       <c r="E3">
+        <v>1.92</v>
+      </c>
+      <c r="F3">
+        <v>1.92</v>
+      </c>
+      <c r="G3">
         <v>8.81</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>13.32</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>0.54</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>2.65</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>0.3</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>0.03</v>
       </c>
-      <c r="K3">
+      <c r="M3">
         <v>0.34</v>
       </c>
+      <c r="N3" s="6"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:14">
       <c r="A4" s="13" t="s">
         <v>91</v>
       </c>
@@ -1184,28 +1700,35 @@
         <v>0.47</v>
       </c>
       <c r="E4">
+        <v>0.47</v>
+      </c>
+      <c r="F4">
+        <v>0.47</v>
+      </c>
+      <c r="G4">
         <v>0.51</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>0.92</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>3.37</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>0.05</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>0</v>
       </c>
-      <c r="K4">
+      <c r="M4">
         <v>0.77</v>
       </c>
+      <c r="N4" s="6"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:14">
       <c r="A5" s="13" t="s">
         <v>92</v>
       </c>
@@ -1219,39 +1742,78 @@
         <v>0.21</v>
       </c>
       <c r="E5">
+        <v>0.21</v>
+      </c>
+      <c r="F5">
+        <v>0.21</v>
+      </c>
+      <c r="G5">
         <v>0.26</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>0.33</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>1.39</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>2.15</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>0.04</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>0</v>
       </c>
-      <c r="K5">
+      <c r="M5">
         <v>0.56000000000000005</v>
       </c>
+      <c r="N5" s="6"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="6"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="6"/>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="6"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7DC8ABB-61B9-4E49-970C-882DDCAD30FD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26B95C06-18D0-B840-B609-1BDFC89B13E0}">
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="A1:K5"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1665,10 +2227,201 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AD2A2BA-2BA1-284D-B683-050BFEF75A5C}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D1:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2">
+        <v>26</v>
+      </c>
+      <c r="C2">
+        <v>3.7</v>
+      </c>
+      <c r="D2">
+        <v>0.75</v>
+      </c>
+      <c r="E2">
+        <v>14.68</v>
+      </c>
+      <c r="F2">
+        <v>21.54</v>
+      </c>
+      <c r="G2">
+        <v>0.44</v>
+      </c>
+      <c r="H2">
+        <v>1.39</v>
+      </c>
+      <c r="I2">
+        <v>0.21</v>
+      </c>
+      <c r="J2">
+        <v>0.04</v>
+      </c>
+      <c r="K2">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3">
+        <v>43.9</v>
+      </c>
+      <c r="C3">
+        <v>10.42</v>
+      </c>
+      <c r="D3">
+        <v>1.92</v>
+      </c>
+      <c r="E3">
+        <v>8.81</v>
+      </c>
+      <c r="F3">
+        <v>13.32</v>
+      </c>
+      <c r="G3">
+        <v>0.54</v>
+      </c>
+      <c r="H3">
+        <v>2.65</v>
+      </c>
+      <c r="I3">
+        <v>0.3</v>
+      </c>
+      <c r="J3">
+        <v>0.03</v>
+      </c>
+      <c r="K3">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4">
+        <v>74.319999999999993</v>
+      </c>
+      <c r="C4">
+        <v>14.76</v>
+      </c>
+      <c r="D4">
+        <v>0.47</v>
+      </c>
+      <c r="E4">
+        <v>0.51</v>
+      </c>
+      <c r="F4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G4">
+        <v>0.92</v>
+      </c>
+      <c r="H4">
+        <v>3.37</v>
+      </c>
+      <c r="I4">
+        <v>0.05</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5">
+        <v>81.08</v>
+      </c>
+      <c r="C5">
+        <v>10.67</v>
+      </c>
+      <c r="D5">
+        <v>0.21</v>
+      </c>
+      <c r="E5">
+        <v>0.26</v>
+      </c>
+      <c r="F5">
+        <v>0.33</v>
+      </c>
+      <c r="G5">
+        <v>1.39</v>
+      </c>
+      <c r="H5">
+        <v>2.15</v>
+      </c>
+      <c r="I5">
+        <v>0.04</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDBA347C-6341-8F47-AC01-0D700C4E65AB}">
   <dimension ref="A1:XEZ20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -8277,7 +9030,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{308B4CB8-955D-D541-A2A4-9BEC8888D421}">
   <dimension ref="A1:L28"/>
   <sheetViews>
@@ -8665,7 +9418,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A90E488-1923-AE4B-B3BC-2420D0E7CEDF}">
   <dimension ref="A1:BC9"/>
   <sheetViews>

</xml_diff>